<commit_message>
removed CommonFuncs -> into DBAddin fixed nonexistent connection exception in DBSetQuery added pivot table creation to Create context Menu moved purgeNames tool into ribbon fixed screenupdating problem when refreshing foreign areas
</commit_message>
<xml_diff>
--- a/test/DBAsyncFunctionsTest.xlsx
+++ b/test/DBAsyncFunctionsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="DBSetQuery" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <definedName name="DBFtarget436755984823148" hidden="1">#REF!</definedName>
     <definedName name="DBFtarget436764557750347" hidden="1">DBRowFetch!$A$2:$H$50</definedName>
     <definedName name="DBFtarget436765432108102" hidden="1">DBListFetch!$A$2:$H$5</definedName>
-    <definedName name="OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" localSheetId="0" hidden="1">DBSetQuery!$A$2:$H$11</definedName>
-    <definedName name="OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht_1" localSheetId="0" hidden="1">DBSetQuery!$A$17:$H$26</definedName>
+    <definedName name="OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" localSheetId="0" hidden="1">DBSetQuery!$A$2:$H$3</definedName>
+    <definedName name="OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht_1" localSheetId="0" hidden="1">DBSetQuery!$A$9:$H$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -28,16 +28,16 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" keepAlive="1" name="OEBFADBPVI00 InfoDB BsGeldwaescheVerdacht" type="5" refreshedVersion="4" background="1" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="select * from employee where fname like 'p%'"/>
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="select * from employee where fname like 'f%'"/>
   </connection>
   <connection id="2" keepAlive="1" name="OEBFADBPVI00 InfoDB BsGeldwaescheVerdacht1" type="5" refreshedVersion="4" saveData="1">
-    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="select * from employee where fname like 'p%'"/>
+    <dbPr connection="Provider=MSDASQL.1;Persist Security Info=True;Extended Properties=&quot;DRIVER=SQL SERVER;SERVER=OEBFADBTVI00;UID=;Trusted_Connection=Yes;APP=Microsoft Office 2010;WSID=00232441EA71;DATABASE=pubs&quot;" command="select * from employee where fname like 'h%'"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t>emp_id</t>
   </si>
@@ -63,129 +63,21 @@
     <t>hire_date</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>0877</t>
   </si>
   <si>
-    <t>1389</t>
-  </si>
-  <si>
     <t>9952</t>
   </si>
   <si>
     <t>9999</t>
   </si>
   <si>
-    <t>PMA42628M</t>
-  </si>
-  <si>
-    <t>Paolo</t>
-  </si>
-  <si>
-    <t>Accorti</t>
-  </si>
-  <si>
-    <t>PSA89086M</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Afonso</t>
-  </si>
-  <si>
-    <t>PTC11962M</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Cramer</t>
-  </si>
-  <si>
-    <t>PHF38899M</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>Franken</t>
-  </si>
-  <si>
-    <t>PXH22250M</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Henriot</t>
-  </si>
-  <si>
-    <t>PDI47470M</t>
-  </si>
-  <si>
-    <t>Palle</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Ibsen</t>
-  </si>
-  <si>
     <t>0736</t>
   </si>
   <si>
-    <t>POK93028M</t>
-  </si>
-  <si>
-    <t>Pirkko</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Koskitalo</t>
-  </si>
-  <si>
-    <t>PCM98509F</t>
-  </si>
-  <si>
-    <t>Patricia</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>McKenna</t>
-  </si>
-  <si>
-    <t>PSP68661F</t>
-  </si>
-  <si>
-    <t>Paula</t>
-  </si>
-  <si>
-    <t>Parente</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>H-B39728F</t>
   </si>
   <si>
@@ -232,6 +124,18 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>F-C16315M</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -337,8 +241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" displayName="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" ref="A2:H11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:H11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" displayName="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht" ref="A2:H3" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A2:H3"/>
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="1" name="emp_id" queryTableFieldId="60"/>
     <tableColumn id="2" uniqueName="2" name="fname" queryTableFieldId="61"/>
@@ -354,8 +258,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3" displayName="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3" ref="A17:H26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A17:H26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3" displayName="Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3" ref="A9:H12" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A9:H12"/>
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="1" name="emp_id" queryTableFieldId="60"/>
     <tableColumn id="2" uniqueName="2" name="fname" queryTableFieldId="61"/>
@@ -657,19 +561,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
@@ -730,11 +633,11 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B1" t="str">
         <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A1,"%"),3,Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht[[#Headers],[emp_id]])</f>
-        <v>Env:Development, statusMsg: Set OLEDB; ListObject to (bgQuery= True): select * from employee where fname like 'p%'</v>
+        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= True): select * from employee where fname like 'f%'</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -765,505 +668,141 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>35</v>
+        <v>227</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1">
-        <v>33843</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <v>33231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>215</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1">
-        <v>32823</v>
+        <v>33180</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>75</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1">
-        <v>33741</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>159</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1">
-        <v>34200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>195</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="1">
-        <v>34098</v>
+      <c r="B6" t="str">
+        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A6,"%"),3,Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3[#Headers])</f>
+        <v>Env:Development, Set OLEDB; ListObject to (bgQuery= False): select * from employee where fname like 'h%'</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>80</v>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1">
-        <v>34302</v>
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1">
-        <v>32721</v>
+        <v>32772</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="1">
-        <v>34353</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="str">
-        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A14,"%"),3,Tabelle_OEBFADBPVI00_InfoDB_BsGeldwaescheVerdacht3[#Headers])</f>
-        <v>Env:Development, statusMsg: Set OLEDB; ListObject to (bgQuery= False): select * from employee where fname like 'p%'</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18">
-        <v>13</v>
-      </c>
-      <c r="F18">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="1">
-        <v>33843</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>34047</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19">
-        <v>14</v>
-      </c>
-      <c r="F19">
-        <v>89</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="1">
-        <v>33231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>215</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1">
-        <v>32823</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>75</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="1">
-        <v>33741</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22">
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <v>159</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="1">
-        <v>34200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="F23">
-        <v>195</v>
-      </c>
-      <c r="G23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="1">
-        <v>34098</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24">
-        <v>80</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="E12">
         <v>12</v>
       </c>
-      <c r="H24" s="1">
-        <v>34302</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25">
-        <v>11</v>
-      </c>
-      <c r="F25">
-        <v>150</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="1">
-        <v>32721</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26">
-        <v>8</v>
-      </c>
-      <c r="F26">
-        <v>125</v>
-      </c>
-      <c r="G26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="1">
-        <v>34353</v>
+      <c r="H12" s="1">
+        <v>32466</v>
       </c>
     </row>
   </sheetData>
@@ -1279,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,11 +829,11 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B1" t="str">
-        <f>_xll.DBRowFetch("select * from employee where fname like "&amp;_xll.DBString(A1,"%"),"",TRUE,A2:H2,A3:H50)</f>
-        <v>Env:Development, statusMsg: Retrieved 1 record from: select * from employee where fname like 'g%'</v>
+        <f>_xll.DBRowFetch("select * from employee where fname like "&amp;_xll.DBString(A1,"%"),3,TRUE,A2:H2,A3:H50)</f>
+        <v>Env:Development, Retrieved 1 record from: select * from employee where fname like 'g%'</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1325,16 +864,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>9</v>
@@ -1516,11 +1055,11 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B1" t="str">
         <f>_xll.DBListFetch("select * from employee where fname like "&amp;_xll.DBString(A1,"%"),3,A2,,,TRUE,TRUE,TRUE)</f>
-        <v>Env:Development, statusMsg: Retrieved 3 records from: select * from employee where fname like 'h%'</v>
+        <v>Env:Development, Retrieved 3 records from: select * from employee where fname like 'h%'</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,16 +1090,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4">
         <v>12</v>
@@ -1569,7 +1108,7 @@
         <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="2">
         <v>32772</v>
@@ -1577,16 +1116,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4">
         <v>7</v>
@@ -1595,7 +1134,7 @@
         <v>120</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2">
         <v>34047</v>
@@ -1603,16 +1142,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4">
         <v>12</v>
@@ -1621,7 +1160,7 @@
         <v>100</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
         <v>32466</v>

</xml_diff>